<commit_message>
update to excel sheet
</commit_message>
<xml_diff>
--- a/Results_reduced_update!!!!!!!new.xlsx
+++ b/Results_reduced_update!!!!!!!new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zmiao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tfry\Desktop\CS522-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAF2B57-CDDE-484B-A7F6-2F7652D83A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715592AC-00A5-4802-9875-2BA31238F554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="1950" windowWidth="18870" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nn (2)" sheetId="3" r:id="rId1"/>
@@ -260,10 +260,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -807,7 +807,7 @@
                   <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>70.5</c:v>
@@ -2347,7 +2347,7 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>75.7</c:v>
@@ -2633,7 +2633,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2646,14 +2646,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>F1-Score</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
               <a:t> Results for All Algorithms with Entire Dataset and Reduced Dataset</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2670,7 +2670,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2732,7 +2732,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2897,7 +2897,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3062,7 +3062,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3136,7 +3136,7 @@
                   <c:v>9.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>73</c:v>
@@ -3192,7 +3192,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3242,7 +3242,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3255,7 +3255,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>F1-Score (%)</a:t>
                 </a:r>
               </a:p>
@@ -3274,7 +3274,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3306,7 +3306,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3334,7 +3334,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3348,7 +3348,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3422,7 +3422,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3435,14 +3435,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2800"/>
               <a:t>Execution</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2800" baseline="0"/>
               <a:t> Time Results for All Algorithms with Entire Dataset and Reduced Dataset</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3459,7 +3459,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3477,7 +3477,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9081109001370735E-2"/>
+          <c:y val="7.2863149337178995E-2"/>
+          <c:w val="0.94298902264088069"/>
+          <c:h val="0.78869722403990483"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -3521,7 +3531,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3686,7 +3696,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3851,7 +3861,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3981,7 +3991,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4031,7 +4041,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4044,15 +4054,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2800"/>
                   <a:t>Execution</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2800" baseline="0"/>
                   <a:t> Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2800"/>
                   <a:t> (sec.)</a:t>
                 </a:r>
               </a:p>
@@ -4071,7 +4081,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4103,7 +4113,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4131,7 +4141,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4145,7 +4155,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4212,9 +4222,79 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Overall Accuracy Results for All Algorithms with Entire Dataset and Reduced Dataset</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.3707905474046306E-2"/>
+          <c:y val="6.2608715908196055E-2"/>
+          <c:w val="0.87050727002893924"/>
+          <c:h val="0.82216221330849693"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -4235,9 +4315,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4274,13 +4352,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4422,7 +4498,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC000"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4439,13 +4515,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4604,13 +4678,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4684,7 +4756,7 @@
                   <c:v>55.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57</c:v>
+                  <c:v>57.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>75.900000000000006</c:v>
@@ -4740,7 +4812,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4790,7 +4862,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4803,7 +4875,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Accuracy (%)</a:t>
                 </a:r>
               </a:p>
@@ -4822,7 +4894,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4854,7 +4926,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4882,7 +4954,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44792573351777853"/>
+          <c:y val="0.96738048619794981"/>
+          <c:w val="0.14878202957510139"/>
+          <c:h val="3.2619513802050158E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4896,7 +4978,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4936,7 +5018,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-US"/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -13556,15 +13638,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>394607</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>379639</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>24493</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13593,16 +13675,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>789215</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>340178</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13631,16 +13713,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>42860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>1114424</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13669,16 +13751,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>2241</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>870856</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123265</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>80683</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>1102178</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14153,13 +14235,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88D8244-74A7-4A2E-A856-40F68AA64FE7}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="B1" s="9" t="s">
         <v>20</v>
       </c>
@@ -14168,7 +14250,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -14365,7 +14447,7 @@
         <v>11.39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -14385,16 +14467,16 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.2" thickBot="1">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:6" ht="16.5" thickBot="1">
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -14472,7 +14554,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" customHeight="1">
+    <row r="19" spans="1:6" ht="17.45" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -14592,7 +14674,7 @@
         <v>1.3009999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1">
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
@@ -14616,16 +14698,16 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.2" thickBot="1">
+    <row r="27" spans="1:6" ht="16.5" thickBot="1">
       <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>0</v>
@@ -14808,22 +14890,22 @@
         <v>11</v>
       </c>
       <c r="B37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="4">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E37" s="4">
-        <v>57</v>
+        <v>57.6</v>
       </c>
       <c r="F37" s="4">
         <v>4.07</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>15</v>
       </c>
@@ -14865,13 +14947,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="B1" s="9" t="s">
         <v>20</v>
       </c>
@@ -15097,16 +15179,16 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -15328,14 +15410,14 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="15.6">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4"/>

</xml_diff>